<commit_message>
revision on main board
</commit_message>
<xml_diff>
--- a/hardware/LM723 voltage regulator-bom.xlsx
+++ b/hardware/LM723 voltage regulator-bom.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\trosh\git\Leadtech-arduino-CSPG\hardware\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -15,11 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="LM723_voltage_regulator" localSheetId="0">Sheet1!$A$1:$H$28</definedName>
+    <definedName name="LM723_voltage_regulator" localSheetId="0">Sheet1!$A$1:$H$29</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -46,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="126">
   <si>
     <t>Qty</t>
   </si>
@@ -255,9 +250,6 @@
     <t>5K</t>
   </si>
   <si>
-    <t>R8, R21</t>
-  </si>
-  <si>
     <t>6.3V</t>
   </si>
   <si>
@@ -397,16 +389,46 @@
   </si>
   <si>
     <t>C433800</t>
+  </si>
+  <si>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t>3362P-1-502LF</t>
+  </si>
+  <si>
+    <t>C81260</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>BOCHEN(Chengdu Guosheng Tech)</t>
+  </si>
+  <si>
+    <t>3362P-1-103</t>
+  </si>
+  <si>
+    <t>C118956</t>
+  </si>
+  <si>
+    <t>3362P-1-500LF</t>
+  </si>
+  <si>
+    <t>C124583</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,12 +437,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -435,10 +463,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,7 +568,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -715,21 +745,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
@@ -742,7 +772,7 @@
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -762,10 +792,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>2</v>
       </c>
@@ -785,11 +815,11 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -810,7 +840,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -828,7 +858,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -845,19 +875,19 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" t="s">
         <v>109</v>
       </c>
-      <c r="H5" t="s">
-        <v>110</v>
-      </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J5" s="1">
         <v>4.875E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1</v>
       </c>
@@ -878,7 +908,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1</v>
       </c>
@@ -898,19 +928,19 @@
         <v>28</v>
       </c>
       <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
         <v>112</v>
       </c>
-      <c r="H7" t="s">
-        <v>113</v>
-      </c>
       <c r="I7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J7" s="1">
         <v>6.0039999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>8</v>
       </c>
@@ -927,19 +957,19 @@
         <v>29</v>
       </c>
       <c r="G8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
         <v>112</v>
       </c>
-      <c r="H8" t="s">
-        <v>113</v>
-      </c>
       <c r="I8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J8" s="1">
         <v>6.0039999999999998E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2</v>
       </c>
@@ -956,19 +986,19 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="1">
         <v>6.0039999999999998E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1</v>
       </c>
@@ -986,7 +1016,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1007,7 +1037,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1025,7 +1055,7 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1046,7 +1076,7 @@
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1067,7 +1097,7 @@
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1088,7 +1118,7 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1106,7 +1136,7 @@
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1124,7 +1154,7 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1141,19 +1171,19 @@
         <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J18" s="1">
         <v>2.101E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1171,202 +1201,256 @@
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:11">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="G20" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.204545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.21060599999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.13120799999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" t="s">
-        <v>74</v>
-      </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="B25" t="s">
         <v>77</v>
       </c>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" t="s">
+        <v>104</v>
+      </c>
+      <c r="I27" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.10634299999999999</v>
+      </c>
+      <c r="K27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
         <v>2</v>
       </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" t="s">
-        <v>81</v>
-      </c>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" t="s">
-        <v>105</v>
-      </c>
-      <c r="I26" t="s">
-        <v>106</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0.10634299999999999</v>
-      </c>
-      <c r="K26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="B29" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
         <v>95</v>
       </c>
-      <c r="C28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E29" t="s">
         <v>96</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F29" t="s">
         <v>97</v>
-      </c>
-      <c r="F28" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>